<commit_message>
Tweak mortality charts to show age 20 upwards
</commit_message>
<xml_diff>
--- a/data/percentage_mortality_covid.xlsx
+++ b/data/percentage_mortality_covid.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416D952A-6D27-437E-8448-C7C02DB0B9D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A67F6CC-B2CC-48D3-9B81-D003EFEEA8C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1114AD08-1D74-4A2B-83BF-3AE2DE711135}"/>
   </bookViews>
@@ -106,8 +106,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="General_)"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -188,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -339,64 +339,52 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0-4</c:v>
+                  <c:v>20-24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5-9</c:v>
+                  <c:v>25-29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10-14</c:v>
+                  <c:v>30-34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15-19</c:v>
+                  <c:v>35-39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20-24</c:v>
+                  <c:v>40-44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25-29</c:v>
+                  <c:v>45-49</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30-34</c:v>
+                  <c:v>50-54</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35-39</c:v>
+                  <c:v>55-59</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40-44</c:v>
+                  <c:v>60-64</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45-49</c:v>
+                  <c:v>65-69</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50-54</c:v>
+                  <c:v>70-74</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55-59</c:v>
+                  <c:v>75-79</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60-64</c:v>
+                  <c:v>80-84</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65-69</c:v>
+                  <c:v>85-89</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70-74</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>75-79</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80-84</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85-89</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>90+</c:v>
                 </c:pt>
               </c:strCache>
@@ -404,65 +392,53 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$20</c:f>
+              <c:f>Sheet1!$D$6:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>5.7717076087555655E-7</c:v>
+                  <c:v>8.9424472226249338E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6867347843492325E-7</c:v>
+                  <c:v>1.4465034395607218E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1315209197002034E-6</c:v>
+                  <c:v>2.7493758916725903E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0650279392621805E-6</c:v>
+                  <c:v>4.414884848064162E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9424472226249338E-6</c:v>
+                  <c:v>9.0405493752115392E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4465034395607218E-5</c:v>
+                  <c:v>1.5428298769516543E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7493758916725903E-5</c:v>
+                  <c:v>2.6720343144439322E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.414884848064162E-5</c:v>
+                  <c:v>4.8455157503695219E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0405493752115392E-5</c:v>
+                  <c:v>8.2761216792629139E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5428298769516543E-4</c:v>
+                  <c:v>1.2944453657445982E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.6720343144439322E-4</c:v>
+                  <c:v>2.1763583734534979E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8455157503695219E-4</c:v>
+                  <c:v>4.498732993110907E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.2761216792629139E-4</c:v>
+                  <c:v>8.5187640306939611E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2944453657445982E-3</c:v>
+                  <c:v>1.4830944159304926E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1763583734534979E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.498732993110907E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.5187640306939611E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.4830944159304926E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>2.6530288121886347E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -893,64 +869,52 @@
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$6:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="19"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0-4</c:v>
+                  <c:v>20-24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5-9</c:v>
+                  <c:v>25-29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10-14</c:v>
+                  <c:v>30-34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15-19</c:v>
+                  <c:v>35-39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20-24</c:v>
+                  <c:v>40-44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25-29</c:v>
+                  <c:v>45-49</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30-34</c:v>
+                  <c:v>50-54</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35-39</c:v>
+                  <c:v>55-59</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40-44</c:v>
+                  <c:v>60-64</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45-49</c:v>
+                  <c:v>65-69</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50-54</c:v>
+                  <c:v>70-74</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55-59</c:v>
+                  <c:v>75-79</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60-64</c:v>
+                  <c:v>80-84</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65-69</c:v>
+                  <c:v>85-89</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70-74</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>75-79</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80-84</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85-89</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>90+</c:v>
                 </c:pt>
               </c:strCache>
@@ -958,65 +922,53 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$20</c:f>
+              <c:f>Sheet1!$D$6:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>5.7717076087555655E-7</c:v>
+                  <c:v>8.9424472226249338E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6867347843492325E-7</c:v>
+                  <c:v>1.4465034395607218E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1315209197002034E-6</c:v>
+                  <c:v>2.7493758916725903E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0650279392621805E-6</c:v>
+                  <c:v>4.414884848064162E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9424472226249338E-6</c:v>
+                  <c:v>9.0405493752115392E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4465034395607218E-5</c:v>
+                  <c:v>1.5428298769516543E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7493758916725903E-5</c:v>
+                  <c:v>2.6720343144439322E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.414884848064162E-5</c:v>
+                  <c:v>4.8455157503695219E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0405493752115392E-5</c:v>
+                  <c:v>8.2761216792629139E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5428298769516543E-4</c:v>
+                  <c:v>1.2944453657445982E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.6720343144439322E-4</c:v>
+                  <c:v>2.1763583734534979E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8455157503695219E-4</c:v>
+                  <c:v>4.498732993110907E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.2761216792629139E-4</c:v>
+                  <c:v>8.5187640306939611E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.2944453657445982E-3</c:v>
+                  <c:v>1.4830944159304926E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1763583734534979E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.498732993110907E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.5187640306939611E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.4830944159304926E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>2.6530288121886347E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1025,7 +977,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-36BC-4B1E-BAE4-F921A1507CD6}"/>
+              <c16:uniqueId val="{00000001-5D2A-4B57-838B-38CB5ED8906C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1192,6 +1144,1101 @@
                 <a:r>
                   <a:rPr lang="en-GB" sz="1050"/>
                   <a:t>% of age group who died from COVID-19 (log scale)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441969656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>Sheet1!$A$22</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Percentage of population who died from COVID-19 in England and Wales
+Weekly deaths registered up to 27 Nov 2020 using ONS data
+Used ONS population estimates from mid-2019</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% of population who have died from COVID-19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:name>Trend (exponential)</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10-14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15-19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20-24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25-29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30-34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35-39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40-44</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45-49</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50-54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55-59</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60-64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65-69</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70-74</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75-79</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80-84</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85-89</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90+</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5.7717076087555655E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6867347843492325E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1315209197002034E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0650279392621805E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9424472226249338E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4465034395607218E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7493758916725903E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.414884848064162E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0405493752115392E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5428298769516543E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6720343144439322E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8455157503695219E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.2761216792629139E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2944453657445982E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.1763583734534979E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.498732993110907E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.5187640306939611E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4830944159304926E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6530288121886347E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D637-42CF-8B48-76CBE1206B69}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="441969656"/>
+        <c:axId val="441973592"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="441969656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1050"/>
+                  <a:t>Age Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441973592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="441973592"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1050"/>
+                  <a:t>% of age group who died from COVID-19 (log scale)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441969656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>Sheet1!$A$22</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Percentage of population who died from COVID-19 in England and Wales
+Weekly deaths registered up to 27 Nov 2020 using ONS data
+Used ONS population estimates from mid-2019</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% of population who have died from COVID-19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10-14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15-19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20-24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25-29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30-34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35-39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40-44</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45-49</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50-54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55-59</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60-64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65-69</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70-74</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75-79</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80-84</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85-89</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90+</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5.7717076087555655E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6867347843492325E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1315209197002034E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0650279392621805E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9424472226249338E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4465034395607218E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7493758916725903E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.414884848064162E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0405493752115392E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5428298769516543E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6720343144439322E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8455157503695219E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.2761216792629139E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2944453657445982E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.1763583734534979E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.498732993110907E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.5187640306939611E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4830944159304926E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6530288121886347E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F46E-4C57-BB65-19BF12B2516E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="441969656"/>
+        <c:axId val="441973592"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="441969656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1050"/>
+                  <a:t>Age Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441973592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="441973592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1050"/>
+                  <a:t>% of age group who have died from COVID-19</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1423,6 +2470,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1940,6 +3067,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2510,10 +4669,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85F1CAB4-DDF0-4AA4-B0D4-58A962431F32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C68CE257-8B15-47C1-BF67-29469973E4DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2528,6 +4687,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>244800</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>129000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8931903-859E-4CDA-9B62-A3D6438AF33C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>244800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>129000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C704B038-BAD3-4E47-A669-3ED384DA2375}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2835,7 +5070,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D8BE8C-7C28-4181-9EFC-88B4F902474A}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2870,7 +5107,7 @@
         <v>3465179</v>
       </c>
       <c r="D2" s="6">
-        <f>B2/C2</f>
+        <f t="shared" ref="D2:D20" si="0">B2/C2</f>
         <v>5.7717076087555655E-7</v>
       </c>
     </row>
@@ -2885,7 +5122,7 @@
         <v>3721990</v>
       </c>
       <c r="D3" s="6">
-        <f>B3/C3</f>
+        <f t="shared" si="0"/>
         <v>2.6867347843492325E-7</v>
       </c>
     </row>
@@ -2900,7 +5137,7 @@
         <v>3535065</v>
       </c>
       <c r="D4" s="6">
-        <f>B4/C4</f>
+        <f t="shared" si="0"/>
         <v>1.1315209197002034E-6</v>
       </c>
     </row>
@@ -2915,7 +5152,7 @@
         <v>3262613</v>
       </c>
       <c r="D5" s="6">
-        <f>B5/C5</f>
+        <f t="shared" si="0"/>
         <v>3.0650279392621805E-6</v>
       </c>
     </row>
@@ -2930,7 +5167,7 @@
         <v>3690265</v>
       </c>
       <c r="D6" s="6">
-        <f>B6/C6</f>
+        <f t="shared" si="0"/>
         <v>8.9424472226249338E-6</v>
       </c>
     </row>
@@ -2945,7 +5182,7 @@
         <v>4009669</v>
       </c>
       <c r="D7" s="6">
-        <f>B7/C7</f>
+        <f t="shared" si="0"/>
         <v>1.4465034395607218E-5</v>
       </c>
     </row>
@@ -2960,7 +5197,7 @@
         <v>4000908</v>
       </c>
       <c r="D8" s="6">
-        <f>B8/C8</f>
+        <f t="shared" si="0"/>
         <v>2.7493758916725903E-5</v>
       </c>
     </row>
@@ -2975,7 +5212,7 @@
         <v>3918562</v>
       </c>
       <c r="D9" s="6">
-        <f>B9/C9</f>
+        <f t="shared" si="0"/>
         <v>4.414884848064162E-5</v>
       </c>
     </row>
@@ -2990,7 +5227,7 @@
         <v>3583853</v>
       </c>
       <c r="D10" s="6">
-        <f>B10/C10</f>
+        <f t="shared" si="0"/>
         <v>9.0405493752115392E-5</v>
       </c>
     </row>
@@ -3005,7 +5242,7 @@
         <v>3914884</v>
       </c>
       <c r="D11" s="6">
-        <f>B11/C11</f>
+        <f t="shared" si="0"/>
         <v>1.5428298769516543E-4</v>
       </c>
     </row>
@@ -3020,7 +5257,7 @@
         <v>4127941</v>
       </c>
       <c r="D12" s="6">
-        <f>B12/C12</f>
+        <f t="shared" si="0"/>
         <v>2.6720343144439322E-4</v>
       </c>
     </row>
@@ -3035,7 +5272,7 @@
         <v>3888131</v>
       </c>
       <c r="D13" s="6">
-        <f>B13/C13</f>
+        <f t="shared" si="0"/>
         <v>4.8455157503695219E-4</v>
       </c>
     </row>
@@ -3050,7 +5287,7 @@
         <v>3304688</v>
       </c>
       <c r="D14" s="6">
-        <f>B14/C14</f>
+        <f t="shared" si="0"/>
         <v>8.2761216792629139E-4</v>
       </c>
     </row>
@@ -3065,7 +5302,7 @@
         <v>2978882</v>
       </c>
       <c r="D15" s="6">
-        <f>B15/C15</f>
+        <f t="shared" si="0"/>
         <v>1.2944453657445982E-3</v>
       </c>
     </row>
@@ -3080,7 +5317,7 @@
         <v>2958612</v>
       </c>
       <c r="D16" s="6">
-        <f>B16/C16</f>
+        <f t="shared" si="0"/>
         <v>2.1763583734534979E-3</v>
       </c>
     </row>
@@ -3095,7 +5332,7 @@
         <v>2067471</v>
       </c>
       <c r="D17" s="6">
-        <f>B17/C17</f>
+        <f t="shared" si="0"/>
         <v>4.498732993110907E-3</v>
       </c>
     </row>
@@ -3110,7 +5347,7 @@
         <v>1529682</v>
       </c>
       <c r="D18" s="6">
-        <f>B18/C18</f>
+        <f t="shared" si="0"/>
         <v>8.5187640306939611E-3</v>
       </c>
     </row>
@@ -3125,7 +5362,7 @@
         <v>933656</v>
       </c>
       <c r="D19" s="6">
-        <f>B19/C19</f>
+        <f t="shared" si="0"/>
         <v>1.4830944159304926E-2</v>
       </c>
     </row>
@@ -3140,7 +5377,7 @@
         <v>547789</v>
       </c>
       <c r="D20" s="6">
-        <f>B20/C20</f>
+        <f t="shared" si="0"/>
         <v>2.6530288121886347E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final wording of mortality charts tweaked
</commit_message>
<xml_diff>
--- a/data/percentage_mortality_covid.xlsx
+++ b/data/percentage_mortality_covid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49607C8-71AF-417A-BB1F-3494FFAA98CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7D77A8-F429-4C5C-9E6C-905A7CEBD624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1114AD08-1D74-4A2B-83BF-3AE2DE711135}"/>
   </bookViews>
@@ -5070,8 +5070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D8BE8C-7C28-4181-9EFC-88B4F902474A}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>